<commit_message>
Historial cambios y prototipos
</commit_message>
<xml_diff>
--- a/Product Backlog V2 (ultima).xlsx
+++ b/Product Backlog V2 (ultima).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferde\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BD2211-8121-488B-B2F7-25A47158274F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FB937E-6C0A-4880-B5B8-0D0B9D158569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Incrementos-Sprint" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Historias de Usuario'!$B$1:$I$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Historias de Usuario'!$B$1:$I$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="232">
   <si>
     <t>Columna</t>
   </si>
@@ -531,9 +531,6 @@
     <t xml:space="preserve">Finalizar la creación de sprint y la versión final a la persona interesada (nutriologa) y al equipo  en general. </t>
   </si>
   <si>
-    <t>TOTAL HT-06</t>
-  </si>
-  <si>
     <t xml:space="preserve">En proceso  </t>
   </si>
   <si>
@@ -602,9 +599,6 @@
     <t>SPRINT 6 Gestión de Citas con Nutrióloga</t>
   </si>
   <si>
-    <t>SPRINT 11 Implementación de la Capa de Presentación (Interfaz de Usuario)</t>
-  </si>
-  <si>
     <t>Trabaja con nutricionistas y pacientes para definir los requisitos del sistema de gestión de citas, incluyendo la disponibilidad de la nutrióloga, la duración de las citas y la información necesaria del paciente.</t>
   </si>
   <si>
@@ -727,6 +721,40 @@
   </si>
   <si>
     <t>OBSERVACION</t>
+  </si>
+  <si>
+    <t>Desarrollo de prototipado de baja fidelidad con interactividad</t>
+  </si>
+  <si>
+    <t>Prototipado</t>
+  </si>
+  <si>
+    <t>sprint 15</t>
+  </si>
+  <si>
+    <t>La tarea de implementar prototipado de baja fidelidad permite la visualización clara de como ira ubicado cada elemento en la interfaz así como guiarnos con la interactividad planteada.</t>
+  </si>
+  <si>
+    <t>SPRINT 12 Implementación de la Capa de Presentación (Interfaz de Usuario)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Inicia un nuevo proyecto en Balsamiq y define el objetivo del prototipo de baja fidelidad. Selecciona la plataforma objetivo (web) y establece las funciones clave que se deben demostrar en el prototipo. Realizó los modulos de plan de comida</t>
+  </si>
+  <si>
+    <t>Utiliza las herramientas de Balsamiq para crear bosquejos de las diferentes pantallas. Organiza los elementos de la interfaz de usuario y crea un storyboard simple que muestre la secuencia de interacciones. Realiza modulos de gestion de citas, configuracion, login, etc.</t>
+  </si>
+  <si>
+    <t>Utiliza las herramientas de Balsamiq para crear bosquejos de las diferentes pantallas. Organiza los elementos de la interfaz de usuario y crea un storyboard simple que muestre la secuencia de interacciones. Realiza modulos de actividades, historial clinico e historial medidas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utiliza las herramientas de Balsamiq para crear bosquejos de las diferentes pantallas. Organiza los elementos de la interfaz de usuario y crea un storyboard simple que muestre la secuencia de interacciones. Realiza login, pacientes, suscripcion, asignacion suscripcion. </t>
+  </si>
+  <si>
+    <t>Facilitar las reuniones para asegurarse de que todos estén alineados en cuanto a los objetivos del prototipado de baja fidelidad e interactividad. 
+Elimina obstáculos y apoya en la resolución de problemas para garantizar un progreso fluido durante el sprint. Pruebas para verificar la interactividad.</t>
+  </si>
+  <si>
+    <t>SPRINT 11 Desarrollo de prototipado de baja fidelidad con interactividad</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1032,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1097,13 +1125,37 @@
     <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1118,32 +1170,17 @@
     <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1449,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I26"/>
+  <dimension ref="B1:I27"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A10" zoomScale="75" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1874,17 +1911,17 @@
       <c r="B19" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>71</v>
+      <c r="C19" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>222</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>86</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>97</v>
@@ -1892,100 +1929,116 @@
       <c r="H19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="53" t="s">
+    <row r="21" spans="2:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C21" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D21" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="55" t="s">
+      <c r="E21" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="55" t="s">
+      <c r="F21" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="G20" s="55" t="s">
-        <v>150</v>
-      </c>
-      <c r="H20" s="55" t="s">
-        <v>222</v>
-      </c>
-      <c r="I20" s="55" t="s">
+      <c r="G21" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="H21" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="I21" s="42" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>86</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>43</v>
       </c>
       <c r="I22" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-    </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="11"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -1995,7 +2048,7 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="10"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -2013,6 +2066,16 @@
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2128,10 +2191,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC15734A-155F-48CB-B53D-F0BB6E0DBE89}">
-  <dimension ref="A2:J122"/>
+  <dimension ref="A2:J130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="82" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="82" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2144,18 +2207,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -2315,35 +2378,35 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
       <c r="J9" s="34">
         <f>SUM(J4:J8)</f>
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
@@ -2531,35 +2594,35 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="34">
         <f>SUM(J12:J16)</f>
         <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
@@ -2727,52 +2790,52 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
       <c r="J25" s="34">
         <f>SUM(J20:J24)</f>
         <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
       <c r="J26" s="33">
         <f>SUM(J17+J25+J9)</f>
         <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
@@ -2972,35 +3035,35 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
       <c r="J34" s="35">
         <f>SUM(J29:J33)</f>
         <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="45"/>
-      <c r="J35" s="45"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="30" t="s">
@@ -3200,35 +3263,35 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="40" t="s">
-        <v>213</v>
-      </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
+      <c r="A42" s="49" t="s">
+        <v>211</v>
+      </c>
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
       <c r="J42" s="35">
         <f>SUM(J37:J41)</f>
         <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="30" t="s">
@@ -3342,7 +3405,7 @@
         <v>147</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C48" s="25" t="s">
         <v>114</v>
@@ -3388,35 +3451,35 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="40" t="s">
-        <v>214</v>
-      </c>
-      <c r="B50" s="40"/>
-      <c r="C50" s="40"/>
-      <c r="D50" s="40"/>
-      <c r="E50" s="40"/>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40"/>
-      <c r="H50" s="40"/>
-      <c r="I50" s="40"/>
+      <c r="A50" s="49" t="s">
+        <v>212</v>
+      </c>
+      <c r="B50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
       <c r="J50" s="35">
         <f>SUM(J45:J49)</f>
         <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="42" t="s">
+      <c r="A51" s="55" t="s">
         <v>157</v>
       </c>
-      <c r="B51" s="42"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="42"/>
-      <c r="J51" s="42"/>
+      <c r="B51" s="55"/>
+      <c r="C51" s="55"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="55"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="55"/>
+      <c r="I51" s="55"/>
+      <c r="J51" s="55"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="30" t="s">
@@ -3455,7 +3518,7 @@
         <v>57</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C53" s="25" t="s">
         <v>114</v>
@@ -3521,7 +3584,7 @@
         <v>57</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C55" s="25" t="s">
         <v>114</v>
@@ -3554,7 +3617,7 @@
         <v>57</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C56" s="25" t="s">
         <v>114</v>
@@ -3616,35 +3679,35 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="40" t="s">
-        <v>167</v>
-      </c>
-      <c r="B58" s="40"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="40"/>
-      <c r="I58" s="40"/>
+      <c r="A58" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="49"/>
+      <c r="C58" s="49"/>
+      <c r="D58" s="49"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="49"/>
+      <c r="G58" s="49"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="49"/>
       <c r="J58" s="35">
         <f>SUM(J53:J57)</f>
         <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="B59" s="41"/>
-      <c r="C59" s="41"/>
-      <c r="D59" s="41"/>
-      <c r="E59" s="41"/>
-      <c r="F59" s="41"/>
-      <c r="G59" s="41"/>
-      <c r="H59" s="41"/>
-      <c r="I59" s="41"/>
-      <c r="J59" s="41"/>
+      <c r="A59" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" s="50"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="50"/>
+      <c r="H59" s="50"/>
+      <c r="I59" s="50"/>
+      <c r="J59" s="50"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="30" t="s">
@@ -3683,7 +3746,7 @@
         <v>67</v>
       </c>
       <c r="B61" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>114</v>
@@ -3716,7 +3779,7 @@
         <v>67</v>
       </c>
       <c r="B62" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>114</v>
@@ -3749,7 +3812,7 @@
         <v>67</v>
       </c>
       <c r="B63" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C63" s="25" t="s">
         <v>114</v>
@@ -3782,7 +3845,7 @@
         <v>67</v>
       </c>
       <c r="B64" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C64" s="25" t="s">
         <v>114</v>
@@ -3815,7 +3878,7 @@
         <v>67</v>
       </c>
       <c r="B65" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C65" s="25" t="s">
         <v>114</v>
@@ -3844,35 +3907,35 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" s="40" t="s">
-        <v>215</v>
-      </c>
-      <c r="B66" s="40"/>
-      <c r="C66" s="40"/>
-      <c r="D66" s="40"/>
-      <c r="E66" s="40"/>
-      <c r="F66" s="40"/>
-      <c r="G66" s="40"/>
-      <c r="H66" s="40"/>
-      <c r="I66" s="40"/>
+      <c r="A66" s="49" t="s">
+        <v>213</v>
+      </c>
+      <c r="B66" s="49"/>
+      <c r="C66" s="49"/>
+      <c r="D66" s="49"/>
+      <c r="E66" s="49"/>
+      <c r="F66" s="49"/>
+      <c r="G66" s="49"/>
+      <c r="H66" s="49"/>
+      <c r="I66" s="49"/>
       <c r="J66" s="35">
         <f>SUM(J61:J65)</f>
         <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="B67" s="41"/>
-      <c r="C67" s="41"/>
-      <c r="D67" s="41"/>
-      <c r="E67" s="41"/>
-      <c r="F67" s="41"/>
-      <c r="G67" s="41"/>
-      <c r="H67" s="41"/>
-      <c r="I67" s="41"/>
-      <c r="J67" s="41"/>
+      <c r="A67" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="B67" s="50"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="50"/>
+      <c r="E67" s="50"/>
+      <c r="F67" s="50"/>
+      <c r="G67" s="50"/>
+      <c r="H67" s="50"/>
+      <c r="I67" s="50"/>
+      <c r="J67" s="50"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="30" t="s">
@@ -3911,7 +3974,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C69" s="25" t="s">
         <v>114</v>
@@ -3944,7 +4007,7 @@
         <v>66</v>
       </c>
       <c r="B70" s="29" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C70" s="25" t="s">
         <v>114</v>
@@ -3977,7 +4040,7 @@
         <v>66</v>
       </c>
       <c r="B71" s="29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C71" s="25" t="s">
         <v>114</v>
@@ -4010,7 +4073,7 @@
         <v>66</v>
       </c>
       <c r="B72" s="29" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C72" s="25" t="s">
         <v>114</v>
@@ -4043,7 +4106,7 @@
         <v>66</v>
       </c>
       <c r="B73" s="29" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C73" s="25" t="s">
         <v>114</v>
@@ -4072,35 +4135,35 @@
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A74" s="40" t="s">
-        <v>216</v>
-      </c>
-      <c r="B74" s="40"/>
-      <c r="C74" s="40"/>
-      <c r="D74" s="40"/>
-      <c r="E74" s="40"/>
-      <c r="F74" s="40"/>
-      <c r="G74" s="40"/>
-      <c r="H74" s="40"/>
-      <c r="I74" s="40"/>
+      <c r="A74" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B74" s="49"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="49"/>
+      <c r="E74" s="49"/>
+      <c r="F74" s="49"/>
+      <c r="G74" s="49"/>
+      <c r="H74" s="49"/>
+      <c r="I74" s="49"/>
       <c r="J74" s="35">
         <f>SUM(J69:J73)</f>
         <v>160</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75" s="41" t="s">
-        <v>187</v>
-      </c>
-      <c r="B75" s="41"/>
-      <c r="C75" s="41"/>
-      <c r="D75" s="41"/>
-      <c r="E75" s="41"/>
-      <c r="F75" s="41"/>
-      <c r="G75" s="41"/>
-      <c r="H75" s="41"/>
-      <c r="I75" s="41"/>
-      <c r="J75" s="41"/>
+      <c r="A75" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="B75" s="50"/>
+      <c r="C75" s="50"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="50"/>
+      <c r="F75" s="50"/>
+      <c r="G75" s="50"/>
+      <c r="H75" s="50"/>
+      <c r="I75" s="50"/>
+      <c r="J75" s="50"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="30" t="s">
@@ -4139,7 +4202,7 @@
         <v>65</v>
       </c>
       <c r="B77" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C77" s="25" t="s">
         <v>114</v>
@@ -4172,7 +4235,7 @@
         <v>65</v>
       </c>
       <c r="B78" s="29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C78" s="25" t="s">
         <v>114</v>
@@ -4205,7 +4268,7 @@
         <v>65</v>
       </c>
       <c r="B79" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C79" s="25" t="s">
         <v>114</v>
@@ -4238,7 +4301,7 @@
         <v>65</v>
       </c>
       <c r="B80" s="29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C80" s="25" t="s">
         <v>114</v>
@@ -4271,7 +4334,7 @@
         <v>65</v>
       </c>
       <c r="B81" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C81" s="25" t="s">
         <v>114</v>
@@ -4300,35 +4363,35 @@
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A82" s="40" t="s">
-        <v>217</v>
-      </c>
-      <c r="B82" s="40"/>
-      <c r="C82" s="40"/>
-      <c r="D82" s="40"/>
-      <c r="E82" s="40"/>
-      <c r="F82" s="40"/>
-      <c r="G82" s="40"/>
-      <c r="H82" s="40"/>
-      <c r="I82" s="40"/>
+      <c r="A82" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="B82" s="49"/>
+      <c r="C82" s="49"/>
+      <c r="D82" s="49"/>
+      <c r="E82" s="49"/>
+      <c r="F82" s="49"/>
+      <c r="G82" s="49"/>
+      <c r="H82" s="49"/>
+      <c r="I82" s="49"/>
       <c r="J82" s="35">
         <f>SUM(J77:J81)</f>
         <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A83" s="41" t="s">
-        <v>188</v>
-      </c>
-      <c r="B83" s="41"/>
-      <c r="C83" s="41"/>
-      <c r="D83" s="41"/>
-      <c r="E83" s="41"/>
-      <c r="F83" s="41"/>
-      <c r="G83" s="41"/>
-      <c r="H83" s="41"/>
-      <c r="I83" s="41"/>
-      <c r="J83" s="41"/>
+      <c r="A83" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="B83" s="50"/>
+      <c r="C83" s="50"/>
+      <c r="D83" s="50"/>
+      <c r="E83" s="50"/>
+      <c r="F83" s="50"/>
+      <c r="G83" s="50"/>
+      <c r="H83" s="50"/>
+      <c r="I83" s="50"/>
+      <c r="J83" s="50"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="30" t="s">
@@ -4367,7 +4430,7 @@
         <v>64</v>
       </c>
       <c r="B85" s="29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C85" s="25" t="s">
         <v>114</v>
@@ -4400,7 +4463,7 @@
         <v>64</v>
       </c>
       <c r="B86" s="29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C86" s="25" t="s">
         <v>114</v>
@@ -4424,7 +4487,7 @@
         <v>3</v>
       </c>
       <c r="J86" s="22">
-        <f t="shared" ref="J86:J88" si="14">SUM(E86:I86)</f>
+        <f t="shared" ref="J86:J87" si="14">SUM(E86:I86)</f>
         <v>16</v>
       </c>
     </row>
@@ -4433,7 +4496,7 @@
         <v>64</v>
       </c>
       <c r="B87" s="29" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C87" s="25" t="s">
         <v>114</v>
@@ -4466,7 +4529,7 @@
         <v>64</v>
       </c>
       <c r="B88" s="29" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C88" s="25" t="s">
         <v>114</v>
@@ -4499,7 +4562,7 @@
         <v>64</v>
       </c>
       <c r="B89" s="29" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C89" s="25" t="s">
         <v>114</v>
@@ -4528,35 +4591,35 @@
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A90" s="40" t="s">
-        <v>218</v>
-      </c>
-      <c r="B90" s="40"/>
-      <c r="C90" s="40"/>
-      <c r="D90" s="40"/>
-      <c r="E90" s="40"/>
-      <c r="F90" s="40"/>
-      <c r="G90" s="40"/>
-      <c r="H90" s="40"/>
-      <c r="I90" s="40"/>
+      <c r="A90" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="B90" s="49"/>
+      <c r="C90" s="49"/>
+      <c r="D90" s="49"/>
+      <c r="E90" s="49"/>
+      <c r="F90" s="49"/>
+      <c r="G90" s="49"/>
+      <c r="H90" s="49"/>
+      <c r="I90" s="49"/>
       <c r="J90" s="35">
         <f>SUM(J85:J89)</f>
         <v>80</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A91" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="B91" s="41"/>
-      <c r="C91" s="41"/>
-      <c r="D91" s="41"/>
-      <c r="E91" s="41"/>
-      <c r="F91" s="41"/>
-      <c r="G91" s="41"/>
-      <c r="H91" s="41"/>
-      <c r="I91" s="41"/>
-      <c r="J91" s="41"/>
+      <c r="A91" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="B91" s="50"/>
+      <c r="C91" s="50"/>
+      <c r="D91" s="50"/>
+      <c r="E91" s="50"/>
+      <c r="F91" s="50"/>
+      <c r="G91" s="50"/>
+      <c r="H91" s="50"/>
+      <c r="I91" s="50"/>
+      <c r="J91" s="50"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="30" t="s">
@@ -4595,7 +4658,7 @@
         <v>63</v>
       </c>
       <c r="B93" s="29" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C93" s="25" t="s">
         <v>114</v>
@@ -4628,7 +4691,7 @@
         <v>63</v>
       </c>
       <c r="B94" s="29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C94" s="25" t="s">
         <v>114</v>
@@ -4652,7 +4715,7 @@
         <v>7</v>
       </c>
       <c r="J94" s="22">
-        <f t="shared" ref="J94:J96" si="16">SUM(E94:I94)</f>
+        <f t="shared" ref="J94:J95" si="16">SUM(E94:I94)</f>
         <v>32</v>
       </c>
     </row>
@@ -4661,7 +4724,7 @@
         <v>63</v>
       </c>
       <c r="B95" s="29" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C95" s="25" t="s">
         <v>114</v>
@@ -4694,7 +4757,7 @@
         <v>63</v>
       </c>
       <c r="B96" s="29" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C96" s="25" t="s">
         <v>114</v>
@@ -4727,7 +4790,7 @@
         <v>63</v>
       </c>
       <c r="B97" s="29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C97" s="25" t="s">
         <v>114</v>
@@ -4756,35 +4819,35 @@
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A98" s="40" t="s">
-        <v>219</v>
-      </c>
-      <c r="B98" s="40"/>
-      <c r="C98" s="40"/>
-      <c r="D98" s="40"/>
-      <c r="E98" s="40"/>
-      <c r="F98" s="40"/>
-      <c r="G98" s="40"/>
-      <c r="H98" s="40"/>
-      <c r="I98" s="40"/>
+      <c r="A98" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="B98" s="49"/>
+      <c r="C98" s="49"/>
+      <c r="D98" s="49"/>
+      <c r="E98" s="49"/>
+      <c r="F98" s="49"/>
+      <c r="G98" s="49"/>
+      <c r="H98" s="49"/>
+      <c r="I98" s="49"/>
       <c r="J98" s="35">
         <f>SUM(J93:J97)</f>
         <v>160</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A99" s="41" t="s">
-        <v>201</v>
-      </c>
-      <c r="B99" s="41"/>
-      <c r="C99" s="41"/>
-      <c r="D99" s="41"/>
-      <c r="E99" s="41"/>
-      <c r="F99" s="41"/>
-      <c r="G99" s="41"/>
-      <c r="H99" s="41"/>
-      <c r="I99" s="41"/>
-      <c r="J99" s="41"/>
+      <c r="A99" s="50" t="s">
+        <v>199</v>
+      </c>
+      <c r="B99" s="50"/>
+      <c r="C99" s="50"/>
+      <c r="D99" s="50"/>
+      <c r="E99" s="50"/>
+      <c r="F99" s="50"/>
+      <c r="G99" s="50"/>
+      <c r="H99" s="50"/>
+      <c r="I99" s="50"/>
+      <c r="J99" s="50"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="30" t="s">
@@ -4823,7 +4886,7 @@
         <v>61</v>
       </c>
       <c r="B101" s="29" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C101" s="25" t="s">
         <v>114</v>
@@ -4856,7 +4919,7 @@
         <v>61</v>
       </c>
       <c r="B102" s="29" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C102" s="25" t="s">
         <v>114</v>
@@ -4880,7 +4943,7 @@
         <v>7</v>
       </c>
       <c r="J102" s="22">
-        <f t="shared" ref="J102:J104" si="18">SUM(E102:I102)</f>
+        <f t="shared" ref="J102:J103" si="18">SUM(E102:I102)</f>
         <v>32</v>
       </c>
     </row>
@@ -4889,7 +4952,7 @@
         <v>61</v>
       </c>
       <c r="B103" s="29" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C103" s="25" t="s">
         <v>114</v>
@@ -4922,7 +4985,7 @@
         <v>61</v>
       </c>
       <c r="B104" s="29" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C104" s="25" t="s">
         <v>114</v>
@@ -4955,7 +5018,7 @@
         <v>61</v>
       </c>
       <c r="B105" s="29" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C105" s="25" t="s">
         <v>114</v>
@@ -4984,35 +5047,35 @@
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A106" s="40" t="s">
-        <v>220</v>
-      </c>
-      <c r="B106" s="40"/>
-      <c r="C106" s="40"/>
-      <c r="D106" s="40"/>
-      <c r="E106" s="40"/>
-      <c r="F106" s="40"/>
-      <c r="G106" s="40"/>
-      <c r="H106" s="40"/>
-      <c r="I106" s="40"/>
+      <c r="A106" s="49" t="s">
+        <v>218</v>
+      </c>
+      <c r="B106" s="49"/>
+      <c r="C106" s="49"/>
+      <c r="D106" s="49"/>
+      <c r="E106" s="49"/>
+      <c r="F106" s="49"/>
+      <c r="G106" s="49"/>
+      <c r="H106" s="49"/>
+      <c r="I106" s="49"/>
       <c r="J106" s="35">
         <f>SUM(J101:J105)</f>
         <v>160</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A107" s="50" t="s">
-        <v>207</v>
-      </c>
-      <c r="B107" s="51"/>
-      <c r="C107" s="51"/>
-      <c r="D107" s="51"/>
-      <c r="E107" s="51"/>
-      <c r="F107" s="51"/>
-      <c r="G107" s="51"/>
-      <c r="H107" s="51"/>
-      <c r="I107" s="51"/>
-      <c r="J107" s="52"/>
+      <c r="A107" s="43" t="s">
+        <v>205</v>
+      </c>
+      <c r="B107" s="44"/>
+      <c r="C107" s="44"/>
+      <c r="D107" s="44"/>
+      <c r="E107" s="44"/>
+      <c r="F107" s="44"/>
+      <c r="G107" s="44"/>
+      <c r="H107" s="44"/>
+      <c r="I107" s="44"/>
+      <c r="J107" s="45"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="30" t="s">
@@ -5051,7 +5114,7 @@
         <v>62</v>
       </c>
       <c r="B109" s="29" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C109" s="25" t="s">
         <v>114</v>
@@ -5084,7 +5147,7 @@
         <v>62</v>
       </c>
       <c r="B110" s="29" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C110" s="25" t="s">
         <v>114</v>
@@ -5117,7 +5180,7 @@
         <v>62</v>
       </c>
       <c r="B111" s="29" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C111" s="25" t="s">
         <v>114</v>
@@ -5150,7 +5213,7 @@
         <v>62</v>
       </c>
       <c r="B112" s="29" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C112" s="25" t="s">
         <v>114</v>
@@ -5183,7 +5246,7 @@
         <v>62</v>
       </c>
       <c r="B113" s="29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C113" s="25" t="s">
         <v>114</v>
@@ -5212,35 +5275,35 @@
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A114" s="47" t="s">
-        <v>221</v>
-      </c>
-      <c r="B114" s="48"/>
-      <c r="C114" s="48"/>
-      <c r="D114" s="48"/>
-      <c r="E114" s="48"/>
-      <c r="F114" s="48"/>
-      <c r="G114" s="48"/>
-      <c r="H114" s="48"/>
-      <c r="I114" s="49"/>
+      <c r="A114" s="46" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="47"/>
+      <c r="C114" s="47"/>
+      <c r="D114" s="47"/>
+      <c r="E114" s="47"/>
+      <c r="F114" s="47"/>
+      <c r="G114" s="47"/>
+      <c r="H114" s="47"/>
+      <c r="I114" s="48"/>
       <c r="J114" s="35">
         <f>SUM(J109:J113)</f>
         <v>160</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A115" s="50" t="s">
-        <v>181</v>
-      </c>
-      <c r="B115" s="51"/>
-      <c r="C115" s="51"/>
-      <c r="D115" s="51"/>
-      <c r="E115" s="51"/>
-      <c r="F115" s="51"/>
-      <c r="G115" s="51"/>
-      <c r="H115" s="51"/>
-      <c r="I115" s="51"/>
-      <c r="J115" s="52"/>
+      <c r="A115" s="56" t="s">
+        <v>231</v>
+      </c>
+      <c r="B115" s="57"/>
+      <c r="C115" s="57"/>
+      <c r="D115" s="57"/>
+      <c r="E115" s="57"/>
+      <c r="F115" s="57"/>
+      <c r="G115" s="57"/>
+      <c r="H115" s="57"/>
+      <c r="I115" s="57"/>
+      <c r="J115" s="58"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" s="30" t="s">
@@ -5279,10 +5342,10 @@
         <v>52</v>
       </c>
       <c r="B117" s="29" t="s">
-        <v>165</v>
+        <v>226</v>
       </c>
       <c r="C117" s="25" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="D117" s="36" t="s">
         <v>116</v>
@@ -5296,26 +5359,24 @@
       <c r="G117" s="22">
         <v>1</v>
       </c>
-      <c r="H117" s="22">
-        <v>2</v>
-      </c>
+      <c r="H117" s="22"/>
       <c r="I117" s="22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J117" s="22">
         <f>SUM(E117:I117)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" ht="66" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A118" s="24" t="s">
         <v>52</v>
       </c>
       <c r="B118" s="29" t="s">
-        <v>162</v>
+        <v>227</v>
       </c>
       <c r="C118" s="25" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="D118" s="22" t="s">
         <v>118</v>
@@ -5327,50 +5388,42 @@
         <v>1</v>
       </c>
       <c r="G118" s="22">
-        <v>2</v>
-      </c>
-      <c r="H118" s="22">
-        <v>1</v>
-      </c>
-      <c r="I118" s="22">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H118" s="22"/>
+      <c r="I118" s="22"/>
       <c r="J118" s="22">
         <f t="shared" ref="J118:J119" si="22">SUM(E118:I118)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" ht="52.8" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A119" s="24" t="s">
         <v>52</v>
       </c>
       <c r="B119" s="29" t="s">
-        <v>163</v>
+        <v>228</v>
       </c>
       <c r="C119" s="25" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="D119" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="E119" s="22">
-        <v>1</v>
-      </c>
-      <c r="F119" s="22">
-        <v>2</v>
-      </c>
+      <c r="E119" s="22"/>
+      <c r="F119" s="22"/>
       <c r="G119" s="22">
         <v>1</v>
       </c>
       <c r="H119" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I119" s="22">
         <v>2</v>
       </c>
       <c r="J119" s="22">
         <f t="shared" si="22"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
@@ -5378,99 +5431,306 @@
         <v>52</v>
       </c>
       <c r="B120" s="29" t="s">
-        <v>164</v>
+        <v>229</v>
       </c>
       <c r="C120" s="25" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="D120" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="E120" s="22">
-        <v>1</v>
-      </c>
-      <c r="F120" s="22">
-        <v>1</v>
-      </c>
+      <c r="E120" s="22"/>
+      <c r="F120" s="22"/>
       <c r="G120" s="22">
+        <v>1</v>
+      </c>
+      <c r="H120" s="22">
+        <v>1</v>
+      </c>
+      <c r="I120" s="22">
         <v>2</v>
-      </c>
-      <c r="H120" s="22">
-        <v>1</v>
-      </c>
-      <c r="I120" s="22">
-        <v>3</v>
       </c>
       <c r="J120" s="22">
         <f>SUM(E120:I120)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A121" s="24" t="s">
         <v>52</v>
       </c>
       <c r="B121" s="29" t="s">
-        <v>166</v>
+        <v>230</v>
       </c>
       <c r="C121" s="25" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="D121" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="E121" s="22">
-        <v>1</v>
-      </c>
-      <c r="F121" s="22">
-        <v>1</v>
-      </c>
-      <c r="G121" s="22">
-        <v>1</v>
-      </c>
+      <c r="E121" s="22"/>
+      <c r="F121" s="22"/>
+      <c r="G121" s="22"/>
       <c r="H121" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I121" s="22">
         <v>2</v>
       </c>
       <c r="J121" s="22">
         <f t="shared" ref="J121" si="23">SUM(E121:I121)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A122" s="47" t="s">
-        <v>160</v>
-      </c>
-      <c r="B122" s="48"/>
-      <c r="C122" s="48"/>
-      <c r="D122" s="48"/>
-      <c r="E122" s="48"/>
-      <c r="F122" s="48"/>
-      <c r="G122" s="48"/>
-      <c r="H122" s="48"/>
-      <c r="I122" s="49"/>
+      <c r="A122" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="B122" s="47"/>
+      <c r="C122" s="47"/>
+      <c r="D122" s="47"/>
+      <c r="E122" s="47"/>
+      <c r="F122" s="47"/>
+      <c r="G122" s="47"/>
+      <c r="H122" s="47"/>
+      <c r="I122" s="48"/>
       <c r="J122" s="35">
         <f>SUM(J117:J121)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A123" s="43" t="s">
+        <v>225</v>
+      </c>
+      <c r="B123" s="44"/>
+      <c r="C123" s="44"/>
+      <c r="D123" s="44"/>
+      <c r="E123" s="44"/>
+      <c r="F123" s="44"/>
+      <c r="G123" s="44"/>
+      <c r="H123" s="44"/>
+      <c r="I123" s="44"/>
+      <c r="J123" s="45"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A124" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B124" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C124" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D124" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E124" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="F124" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G124" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="H124" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="I124" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="J124" s="32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="66" x14ac:dyDescent="0.3">
+      <c r="A125" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B125" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="C125" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D125" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="E125" s="22">
+        <v>1</v>
+      </c>
+      <c r="F125" s="22">
+        <v>1</v>
+      </c>
+      <c r="G125" s="22">
+        <v>1</v>
+      </c>
+      <c r="H125" s="22">
+        <v>2</v>
+      </c>
+      <c r="I125" s="22">
+        <v>3</v>
+      </c>
+      <c r="J125" s="22">
+        <f>SUM(E125:I125)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" ht="66" x14ac:dyDescent="0.3">
+      <c r="A126" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B126" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C126" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D126" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E126" s="22">
+        <v>2</v>
+      </c>
+      <c r="F126" s="22">
+        <v>1</v>
+      </c>
+      <c r="G126" s="22">
+        <v>2</v>
+      </c>
+      <c r="H126" s="22">
+        <v>1</v>
+      </c>
+      <c r="I126" s="22">
+        <v>2</v>
+      </c>
+      <c r="J126" s="22">
+        <f t="shared" ref="J126:J127" si="24">SUM(E126:I126)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A127" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B127" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C127" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D127" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E127" s="22">
+        <v>1</v>
+      </c>
+      <c r="F127" s="22">
+        <v>2</v>
+      </c>
+      <c r="G127" s="22">
+        <v>1</v>
+      </c>
+      <c r="H127" s="22">
+        <v>2</v>
+      </c>
+      <c r="I127" s="22">
+        <v>2</v>
+      </c>
+      <c r="J127" s="22">
+        <f t="shared" si="24"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A128" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B128" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="C128" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D128" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E128" s="22">
+        <v>1</v>
+      </c>
+      <c r="F128" s="22">
+        <v>1</v>
+      </c>
+      <c r="G128" s="22">
+        <v>2</v>
+      </c>
+      <c r="H128" s="22">
+        <v>1</v>
+      </c>
+      <c r="I128" s="22">
+        <v>3</v>
+      </c>
+      <c r="J128" s="22">
+        <f>SUM(E128:I128)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A129" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B129" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="C129" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D129" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E129" s="22">
+        <v>1</v>
+      </c>
+      <c r="F129" s="22">
+        <v>1</v>
+      </c>
+      <c r="G129" s="22">
+        <v>1</v>
+      </c>
+      <c r="H129" s="22">
+        <v>3</v>
+      </c>
+      <c r="I129" s="22">
+        <v>2</v>
+      </c>
+      <c r="J129" s="22">
+        <f t="shared" ref="J129" si="25">SUM(E129:I129)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A130" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="B130" s="47"/>
+      <c r="C130" s="47"/>
+      <c r="D130" s="47"/>
+      <c r="E130" s="47"/>
+      <c r="F130" s="47"/>
+      <c r="G130" s="47"/>
+      <c r="H130" s="47"/>
+      <c r="I130" s="48"/>
+      <c r="J130" s="35">
+        <f>SUM(J125:J129)</f>
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="A115:J115"/>
-    <mergeCell ref="A122:I122"/>
-    <mergeCell ref="A98:I98"/>
-    <mergeCell ref="A99:J99"/>
-    <mergeCell ref="A106:I106"/>
-    <mergeCell ref="A107:J107"/>
-    <mergeCell ref="A114:I114"/>
-    <mergeCell ref="A83:J83"/>
-    <mergeCell ref="A82:I82"/>
-    <mergeCell ref="A90:I90"/>
-    <mergeCell ref="A91:J91"/>
-    <mergeCell ref="A43:J43"/>
-    <mergeCell ref="A50:I50"/>
+  <mergeCells count="33">
+    <mergeCell ref="A123:J123"/>
+    <mergeCell ref="A130:I130"/>
     <mergeCell ref="A42:I42"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A17:I17"/>
@@ -5482,6 +5742,12 @@
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A27:J27"/>
     <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A83:J83"/>
+    <mergeCell ref="A82:I82"/>
+    <mergeCell ref="A90:I90"/>
+    <mergeCell ref="A91:J91"/>
+    <mergeCell ref="A43:J43"/>
+    <mergeCell ref="A50:I50"/>
     <mergeCell ref="A74:I74"/>
     <mergeCell ref="A75:J75"/>
     <mergeCell ref="A51:J51"/>
@@ -5489,13 +5755,20 @@
     <mergeCell ref="A59:J59"/>
     <mergeCell ref="A66:I66"/>
     <mergeCell ref="A67:J67"/>
+    <mergeCell ref="A115:J115"/>
+    <mergeCell ref="A122:I122"/>
+    <mergeCell ref="A98:I98"/>
+    <mergeCell ref="A99:J99"/>
+    <mergeCell ref="A106:I106"/>
+    <mergeCell ref="A107:J107"/>
+    <mergeCell ref="A114:I114"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11 C28 C19 C3 C36 C44 C52 C60 C68 C76 C84 C92 C100 C108 C116" xr:uid="{929D530A-A9D8-4A36-B321-577C73DFDE3C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11 C28 C19 C3 C36 C44 C52 C60 C68 C76 C84 C92 C100 C108 C124 C116" xr:uid="{929D530A-A9D8-4A36-B321-577C73DFDE3C}">
       <formula1>$K$12:$K$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11 D3 D28 D19 D36 D44 D52 D60 D68 D76 D84 D92 D100 D108 D116" xr:uid="{D28816CB-B437-448A-BFD1-A14CE206D049}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11 D3 D28 D19 D36 D44 D52 D60 D68 D76 D84 D92 D100 D108 D116 D124" xr:uid="{D28816CB-B437-448A-BFD1-A14CE206D049}">
       <formula1>$D$12:$D$16</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>